<commit_message>
Feat : Build 아이템 총 정리
</commit_message>
<xml_diff>
--- a/ExcelDB/BuildItemSheet.xlsx
+++ b/ExcelDB/BuildItemSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajin\Desktop\Unity\Unity_project\TeamProject_Survival\Survival\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26288B8A-4E1A-4D43-B90C-FE159EE8BDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665E4BCC-FE84-4F4F-9CB9-C470B60E4980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{87CC9680-1ADE-4891-8706-9F68FAE83D61}"/>
+    <workbookView xWindow="-22644" yWindow="792" windowWidth="21000" windowHeight="12120" xr2:uid="{87CC9680-1ADE-4891-8706-9F68FAE83D61}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildItemData" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Id</t>
   </si>
@@ -89,10 +89,22 @@
     <t>침대 밖은 위험해</t>
   </si>
   <si>
-    <t>Sprites/well</t>
-  </si>
-  <si>
-    <t>Prefabs/BuildItemPrefabs/well</t>
+    <t>Sprites/Table</t>
+  </si>
+  <si>
+    <t>Prefabs/BuildItemPrefabs/Table</t>
+  </si>
+  <si>
+    <t>Sprites/Cabin</t>
+  </si>
+  <si>
+    <t>Prefabs/BuildItemPrefabs/Cabin</t>
+  </si>
+  <si>
+    <t>Sprites/Bed</t>
+  </si>
+  <si>
+    <t>Prefabs/BuildItemPrefabs/Bed</t>
   </si>
 </sst>
 </file>
@@ -479,7 +491,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -573,10 +585,10 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
@@ -602,10 +614,10 @@
         <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>